<commit_message>
README and  xlsx files updated
</commit_message>
<xml_diff>
--- a/UserPrivilege.xlsx
+++ b/UserPrivilege.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VijayanD\Venzo\UserPrivilegesService\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7E0856-4747-4823-915D-C817275C1D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conceptual Design" sheetId="7" r:id="rId1"/>
@@ -22,7 +23,6 @@
     <sheet name="Sheet3" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>PRIVILEGE_ID  </t>
-  </si>
-  <si>
-    <t>https://github.com/VijayanDev/UserRolePrivilege/tree/main/UserPrivilegesService</t>
   </si>
   <si>
     <t>Many To Many</t>
@@ -363,11 +360,14 @@
   <si>
     <t>*We can use Spring framework alone without Spring Boot.But, we need to manage configurations, dependencies build deplyments manually.</t>
   </si>
+  <si>
+    <t>https://github.com/VijayanDev/takehometest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -470,7 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -751,10 +750,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -768,53 +767,53 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,240 +821,240 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
       <c r="C19" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
       <c r="C20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1127,7 +1126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1175,7 +1174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1225,7 +1224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1276,7 +1275,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -1286,7 +1285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1349,7 +1348,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1358,18 +1357,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1378,7 +1377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>